<commit_message>
updated Water Depth for Pioneer MOAS
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL388_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL388_00003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4080" windowWidth="23040" windowHeight="9520" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="41940" yWindow="3960" windowWidth="23040" windowHeight="9520" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1079,7 +1079,7 @@
         <v>29</v>
       </c>
       <c r="J2" s="28">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>26</v>
@@ -1119,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>